<commit_message>
Initial Implementation of Data preprocessing and Rule to P-Value
</commit_message>
<xml_diff>
--- a/csv/priority_results.xlsx
+++ b/csv/priority_results.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackhou\Documents\mri_project\mri_app\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{41BE4CE7-1712-43B7-A7F3-7F321EE0A148}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E85D42-DB13-4CD3-8C8D-E1223890BD49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5316"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rule_results" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="168">
   <si>
     <t>{"Req # CIO": 151695, "height": 168.0, "weight": 78.0, "Sex": "M", "age": 0, "Preferred MRI Site": "RH", "Radiologist Priority": "P3", "medical_condition": ["lump ankle"], "diagnosis": [], "anatomy": ["ankle"], "symptoms": [], "phrases": ["lump", "anterior ankle"], "other_info": []}</t>
   </si>
@@ -518,12 +518,18 @@
   </si>
   <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t>data_results TABLE</t>
+  </si>
+  <si>
+    <t>mri_rules TABLE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -660,7 +666,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -840,8 +846,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -956,6 +974,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1001,9 +1099,37 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1369,2483 +1495,2658 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="30.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" customWidth="1"/>
-    <col min="6" max="6" width="20.77734375" customWidth="1"/>
-    <col min="8" max="8" width="30.77734375" customWidth="1"/>
+    <col min="3" max="3" width="100.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>151695</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="D3" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>129999</v>
       </c>
-      <c r="B3">
-        <v>165</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="2">
+        <v>165</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>165</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D4" s="7">
+        <v>165</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="G4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="I4" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>134203</v>
       </c>
-      <c r="B4">
-        <v>165</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B5" s="2">
+        <v>165</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4">
-        <v>165</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D5" s="7">
+        <v>165</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="G5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="I5" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>156374</v>
       </c>
-      <c r="B5">
+      <c r="B6" s="2">
         <v>236</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5">
+      <c r="D6" s="7">
         <v>236</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="I6" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>159638</v>
       </c>
-      <c r="B6">
+      <c r="B7" s="2">
         <v>236</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6">
+      <c r="D7" s="7">
         <v>236</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="I7" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>163232</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="2">
         <v>120</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D7">
+      <c r="D8" s="7">
         <v>120</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="I8" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>141736</v>
       </c>
-      <c r="B8">
+      <c r="B9" s="2">
         <v>206</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D8">
+      <c r="D9" s="7">
         <v>206</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="I9" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>142943</v>
       </c>
-      <c r="B9">
+      <c r="B10" s="2">
         <v>193</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D9">
+      <c r="D10" s="7">
         <v>193</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="G10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="I10" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>139609</v>
       </c>
-      <c r="B10">
+      <c r="B11" s="2">
         <v>204</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D10">
+      <c r="D11" s="7">
         <v>204</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="G11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="I11" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>140359</v>
       </c>
-      <c r="B11">
+      <c r="B12" s="2">
         <v>193</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D11">
+      <c r="D12" s="7">
         <v>193</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="G12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="I12" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>124652</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="D13" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="16"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>134728</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D13" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="D14" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="16"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
         <v>127661</v>
       </c>
-      <c r="B14">
+      <c r="B15" s="2">
         <v>2</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D14">
+      <c r="D15" s="7">
         <v>2</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I15" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
         <v>137025</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="D16" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
         <v>162919</v>
       </c>
-      <c r="B16">
+      <c r="B17" s="2">
         <v>234</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D16">
+      <c r="D17" s="7">
         <v>234</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G16" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="G17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="I17" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
         <v>122912</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D17" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="D18" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
         <v>137824</v>
       </c>
-      <c r="B18">
+      <c r="B19" s="2">
         <v>134</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D18">
+      <c r="D19" s="7">
         <v>134</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I19" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
         <v>136738</v>
       </c>
-      <c r="B19">
+      <c r="B20" s="2">
         <v>99</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D19">
+      <c r="D20" s="7">
         <v>99</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I19">
+      <c r="I20" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
         <v>160933</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="B21" s="2"/>
+      <c r="C21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D20" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="D21" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
         <v>147842</v>
       </c>
-      <c r="B21">
+      <c r="B22" s="2">
         <v>39</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D21">
+      <c r="D22" s="7">
         <v>39</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F22" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G22" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="I22" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
         <v>162911</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D22" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="D23" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="16"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
         <v>130750</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D23" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="D24" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
         <v>135821</v>
       </c>
-      <c r="B24">
-        <v>165</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="B25" s="2">
+        <v>165</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D24">
-        <v>165</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="D25" s="7">
+        <v>165</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="G25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="I25" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
         <v>164302</v>
       </c>
-      <c r="B25">
+      <c r="B26" s="2">
         <v>204</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D25">
+      <c r="D26" s="7">
         <v>204</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E26" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G25" t="s">
-        <v>4</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="G26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="I26" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
         <v>155198</v>
       </c>
-      <c r="B26">
-        <v>165</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="B27" s="2">
+        <v>165</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D26">
-        <v>165</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="D27" s="7">
+        <v>165</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G26" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="G27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="I27" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
         <v>112707</v>
       </c>
-      <c r="B27">
+      <c r="B28" s="2">
         <v>95</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D27">
+      <c r="D28" s="7">
         <v>95</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E28" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H28" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I28" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
         <v>151564</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="B29" s="2"/>
+      <c r="C29" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D28" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="D29" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="16"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
         <v>139014</v>
       </c>
-      <c r="B29">
+      <c r="B30" s="2">
         <v>234</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D29">
+      <c r="D30" s="7">
         <v>234</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G29" t="s">
-        <v>4</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="G30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="I30" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
         <v>140342</v>
       </c>
-      <c r="B30">
-        <v>165</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="B31" s="2">
+        <v>165</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D30">
-        <v>165</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D31" s="7">
+        <v>165</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F31" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G30" t="s">
-        <v>4</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="G31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="I31" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
         <v>125693</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="B32" s="2"/>
+      <c r="C32" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D31" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32">
+      <c r="D32" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="16"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
         <v>158947</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="B33" s="2"/>
+      <c r="C33" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D32" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33">
+      <c r="D33" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="16"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
         <v>133269</v>
       </c>
-      <c r="B33">
+      <c r="B34" s="2">
         <v>99</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D33">
+      <c r="D34" s="7">
         <v>99</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E34" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F34" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G34" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H34" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I33">
+      <c r="I34" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
         <v>142605</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="B35" s="2"/>
+      <c r="C35" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D34" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="D35" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="16"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
         <v>160382</v>
       </c>
-      <c r="B35">
-        <v>165</v>
-      </c>
-      <c r="C35" s="1" t="s">
+      <c r="B36" s="2">
+        <v>165</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D35">
-        <v>165</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D36" s="7">
+        <v>165</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F36" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G35" t="s">
-        <v>4</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="G36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I35">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="I36" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
         <v>114069</v>
       </c>
-      <c r="B36">
+      <c r="B37" s="2">
         <v>234</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D36">
+      <c r="D37" s="7">
         <v>234</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G36" t="s">
-        <v>4</v>
-      </c>
-      <c r="H36" t="s">
+      <c r="G37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37">
+      <c r="I37" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
         <v>19639</v>
       </c>
-      <c r="B37">
+      <c r="B38" s="2">
         <v>167</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D37">
+      <c r="D38" s="7">
         <v>167</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F38" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G38" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H38" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I37">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="I38" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
         <v>106610</v>
       </c>
-      <c r="B38">
+      <c r="B39" s="2">
         <v>69</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C39" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D38">
+      <c r="D39" s="7">
         <v>69</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G39" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H39" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I39" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
         <v>156190</v>
       </c>
-      <c r="B39">
+      <c r="B40" s="2">
         <v>236</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D39">
+      <c r="D40" s="7">
         <v>236</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E40" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F40" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G40" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H40" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I39">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40">
+      <c r="I40" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
         <v>59831</v>
       </c>
-      <c r="B40">
-        <v>165</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="B41" s="2">
+        <v>165</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D40">
-        <v>165</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="D41" s="7">
+        <v>165</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F41" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G40" t="s">
-        <v>4</v>
-      </c>
-      <c r="H40" t="s">
+      <c r="G41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I40">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41">
+      <c r="I41" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
         <v>154596</v>
       </c>
-      <c r="B41">
+      <c r="B42" s="2">
         <v>193</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D41">
+      <c r="D42" s="7">
         <v>193</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E42" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F42" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G41" t="s">
-        <v>4</v>
-      </c>
-      <c r="H41" t="s">
+      <c r="G42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I41">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42">
+      <c r="I42" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
         <v>96339</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="B43" s="2"/>
+      <c r="C43" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D42" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43">
+      <c r="D43" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="16"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
         <v>103492</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="B44" s="2"/>
+      <c r="C44" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D43" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44">
+      <c r="D44" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="16"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
         <v>151770</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="B45" s="2"/>
+      <c r="C45" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D44" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45">
+      <c r="D45" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="16"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
         <v>135019</v>
       </c>
-      <c r="B45">
+      <c r="B46" s="2">
         <v>193</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D45">
+      <c r="D46" s="7">
         <v>193</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E46" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F46" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G45" t="s">
-        <v>4</v>
-      </c>
-      <c r="H45" t="s">
+      <c r="G46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H46" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46">
+      <c r="I46" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
         <v>156185</v>
       </c>
-      <c r="B46">
+      <c r="B47" s="2">
         <v>206</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D46">
+      <c r="D47" s="7">
         <v>206</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E47" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F47" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G47" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H47" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I46">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47">
+      <c r="I47" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
         <v>143763</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="B48" s="2"/>
+      <c r="C48" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D47" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48">
+      <c r="D48" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="16"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
         <v>155747</v>
       </c>
-      <c r="B48">
+      <c r="B49" s="2">
         <v>206</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D48">
+      <c r="D49" s="7">
         <v>206</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F49" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H49" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I48">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49">
+      <c r="I49" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
         <v>106125</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="B50" s="2"/>
+      <c r="C50" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D49" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50">
+      <c r="D50" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="16"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
         <v>121827</v>
       </c>
-      <c r="B50">
+      <c r="B51" s="2">
         <v>167</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D50">
+      <c r="D51" s="7">
         <v>167</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E51" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F51" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G51" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H51" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I50">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51">
+      <c r="I51" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
         <v>122606</v>
       </c>
-      <c r="B51">
+      <c r="B52" s="2">
         <v>134</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D51">
+      <c r="D52" s="7">
         <v>134</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E52" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G52" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H52" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I52" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
         <v>158843</v>
       </c>
-      <c r="B52">
+      <c r="B53" s="2">
         <v>233</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C53" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D52">
+      <c r="D53" s="7">
         <v>233</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E53" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F53" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G53" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H53" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I53" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
         <v>131946</v>
       </c>
-      <c r="B53">
+      <c r="B54" s="2">
         <v>195</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C54" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D53">
+      <c r="D54" s="7">
         <v>195</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E54" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F54" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G54" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I53">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54">
+      <c r="I54" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
         <v>131196</v>
       </c>
-      <c r="B54">
-        <v>165</v>
-      </c>
-      <c r="C54" s="1" t="s">
+      <c r="B55" s="2">
+        <v>165</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D54">
-        <v>165</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="D55" s="7">
+        <v>165</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F55" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G54" t="s">
-        <v>4</v>
-      </c>
-      <c r="H54" t="s">
+      <c r="G55" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I54">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55">
+      <c r="I55" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
         <v>158585</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="B56" s="2"/>
+      <c r="C56" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D55" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56">
+      <c r="D56" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="16"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
         <v>117377</v>
       </c>
-      <c r="B56">
+      <c r="B57" s="2">
         <v>121</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C57" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D56">
+      <c r="D57" s="7">
         <v>121</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F57" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G57" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H57" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="I56">
+      <c r="I57" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
         <v>120091</v>
       </c>
-      <c r="B57">
+      <c r="B58" s="2">
         <v>167</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C58" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D57">
+      <c r="D58" s="7">
         <v>167</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E58" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F58" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G58" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H57" t="s">
+      <c r="H58" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I57">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58">
+      <c r="I58" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
         <v>81119</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="B59" s="2"/>
+      <c r="C59" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D58" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59">
+      <c r="D59" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="16"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
         <v>58962</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="B60" s="2"/>
+      <c r="C60" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D59" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60">
+      <c r="D60" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="16"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
         <v>118553</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="B61" s="2"/>
+      <c r="C61" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D60" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61">
+      <c r="D61" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="16"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
         <v>134418</v>
       </c>
-      <c r="B61">
+      <c r="B62" s="2">
         <v>199</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C62" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D61">
+      <c r="D62" s="7">
         <v>199</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E62" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F62" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G62" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H62" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I61">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62">
+      <c r="I62" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="7">
         <v>120777</v>
       </c>
-      <c r="B62">
+      <c r="B63" s="2">
         <v>120</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C63" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D62">
+      <c r="D63" s="7">
         <v>120</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F63" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G63" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H62" t="s">
+      <c r="H63" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I62">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63">
+      <c r="I63" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="7">
         <v>155661</v>
       </c>
-      <c r="B63">
+      <c r="B64" s="2">
         <v>206</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C64" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D63">
+      <c r="D64" s="7">
         <v>206</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E64" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F64" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G64" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H64" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I63">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64">
+      <c r="I64" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="7">
         <v>145206</v>
       </c>
-      <c r="B64">
+      <c r="B65" s="2">
         <v>167</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C65" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D64">
+      <c r="D65" s="7">
         <v>167</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E65" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F65" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G65" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H65" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I64">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65">
+      <c r="I65" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="7">
         <v>148368</v>
       </c>
-      <c r="B65">
+      <c r="B66" s="2">
         <v>101</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C66" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D65">
+      <c r="D66" s="7">
         <v>101</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E66" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F66" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G66" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H65" t="s">
+      <c r="H66" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I65" t="s">
+      <c r="I66" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="7">
         <v>132355</v>
       </c>
-      <c r="B66">
+      <c r="B67" s="2">
         <v>234</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C67" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D66">
+      <c r="D67" s="7">
         <v>234</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E67" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F67" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G66" t="s">
-        <v>4</v>
-      </c>
-      <c r="H66" t="s">
+      <c r="G67" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H67" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I66">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67">
+      <c r="I67" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="7">
         <v>151966</v>
       </c>
-      <c r="B67">
+      <c r="B68" s="2">
         <v>234</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C68" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D67">
+      <c r="D68" s="7">
         <v>234</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E68" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F68" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G67" t="s">
-        <v>4</v>
-      </c>
-      <c r="H67" t="s">
+      <c r="G68" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H68" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I67">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68">
+      <c r="I68" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="7">
         <v>144071</v>
       </c>
-      <c r="B68">
+      <c r="B69" s="2">
         <v>51</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C69" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D68">
+      <c r="D69" s="7">
         <v>51</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E69" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F69" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G69" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H69" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="I68">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69">
+      <c r="I69" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="7">
         <v>144108</v>
       </c>
-      <c r="B69">
+      <c r="B70" s="2">
         <v>134</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C70" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D69">
+      <c r="D70" s="7">
         <v>134</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E70" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G70" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H70" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I69" t="s">
+      <c r="I70" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="7">
         <v>140443</v>
       </c>
-      <c r="B70">
+      <c r="B71" s="2">
         <v>199</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C71" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D70">
+      <c r="D71" s="7">
         <v>199</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E71" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F71" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G71" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H71" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I70">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71">
+      <c r="I71" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="7">
         <v>128245</v>
       </c>
-      <c r="B71">
+      <c r="B72" s="2">
         <v>203</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C72" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D71">
+      <c r="D72" s="7">
         <v>203</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E72" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F72" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G72" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H71" t="s">
+      <c r="H72" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I71" t="s">
+      <c r="I72" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="7">
         <v>29629</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="B73" s="2"/>
+      <c r="C73" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D72" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73">
+      <c r="D73" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="16"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="7">
         <v>131486</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="B74" s="2"/>
+      <c r="C74" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D73" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74">
+      <c r="D74" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="16"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="7">
         <v>139750</v>
       </c>
-      <c r="B74">
+      <c r="B75" s="2">
         <v>140</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C75" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D74">
+      <c r="D75" s="7">
         <v>140</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E75" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F75" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G74" t="s">
+      <c r="G75" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H74" t="s">
+      <c r="H75" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="I74">
+      <c r="I75" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="7">
         <v>96961</v>
       </c>
-      <c r="B75">
+      <c r="B76" s="2">
         <v>234</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C76" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D75">
+      <c r="D76" s="7">
         <v>234</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E76" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F76" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G75" t="s">
-        <v>4</v>
-      </c>
-      <c r="H75" t="s">
+      <c r="G76" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H76" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I75">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76">
+      <c r="I76" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="7">
         <v>116766</v>
       </c>
-      <c r="B76">
+      <c r="B77" s="2">
         <v>120</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C77" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D76">
+      <c r="D77" s="7">
         <v>120</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E77" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F77" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G76" t="s">
+      <c r="G77" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H76" t="s">
+      <c r="H77" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I76">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77">
+      <c r="I77" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="7">
         <v>127543</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="B78" s="2"/>
+      <c r="C78" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D77" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78">
+      <c r="D78" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="16"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="7">
         <v>127577</v>
       </c>
-      <c r="B78">
+      <c r="B79" s="2">
         <v>134</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C79" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D78">
+      <c r="D79" s="7">
         <v>134</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E79" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F79" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G79" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H78" t="s">
+      <c r="H79" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I78" t="s">
+      <c r="I79" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="7">
         <v>113567</v>
       </c>
-      <c r="B79">
+      <c r="B80" s="2">
         <v>195</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C80" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D79">
+      <c r="D80" s="7">
         <v>195</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E80" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F80" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G79" t="s">
+      <c r="G80" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H79" t="s">
+      <c r="H80" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I79">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80">
+      <c r="I80" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="7">
         <v>99594</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="B81" s="2"/>
+      <c r="C81" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D80" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81">
+      <c r="D81" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="16"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="7">
         <v>97694</v>
       </c>
-      <c r="B81">
+      <c r="B82" s="2">
         <v>234</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C82" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D81">
+      <c r="D82" s="7">
         <v>234</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E82" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F82" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G81" t="s">
-        <v>4</v>
-      </c>
-      <c r="H81" t="s">
+      <c r="G82" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H82" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I81">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82">
+      <c r="I82" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="7">
         <v>75850</v>
       </c>
-      <c r="B82">
-        <v>165</v>
-      </c>
-      <c r="C82" s="1" t="s">
+      <c r="B83" s="2">
+        <v>165</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D82">
-        <v>165</v>
-      </c>
-      <c r="E82" t="s">
+      <c r="D83" s="7">
+        <v>165</v>
+      </c>
+      <c r="E83" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F83" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G82" t="s">
-        <v>4</v>
-      </c>
-      <c r="H82" t="s">
+      <c r="G83" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H83" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I82">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83">
+      <c r="I83" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="7">
         <v>121503</v>
       </c>
-      <c r="B83">
-        <v>165</v>
-      </c>
-      <c r="C83" s="1" t="s">
+      <c r="B84" s="2">
+        <v>165</v>
+      </c>
+      <c r="C84" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D83">
-        <v>165</v>
-      </c>
-      <c r="E83" t="s">
+      <c r="D84" s="7">
+        <v>165</v>
+      </c>
+      <c r="E84" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F84" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G83" t="s">
-        <v>4</v>
-      </c>
-      <c r="H83" t="s">
+      <c r="G84" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H84" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I83">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84">
+      <c r="I84" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="7">
         <v>154721</v>
       </c>
-      <c r="B84">
+      <c r="B85" s="2">
         <v>192</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C85" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D84">
+      <c r="D85" s="7">
         <v>192</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E85" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F85" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G85" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H85" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I85" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="7">
         <v>125397</v>
       </c>
-      <c r="B85">
+      <c r="B86" s="2">
         <v>207</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C86" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D85">
+      <c r="D86" s="7">
         <v>207</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E86" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F86" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G86" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H85" t="s">
+      <c r="H86" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I85">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86">
+      <c r="I86" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="7">
         <v>104541</v>
       </c>
-      <c r="B86">
-        <v>165</v>
-      </c>
-      <c r="C86" s="1" t="s">
+      <c r="B87" s="2">
+        <v>165</v>
+      </c>
+      <c r="C87" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="D86">
-        <v>165</v>
-      </c>
-      <c r="E86" t="s">
+      <c r="D87" s="7">
+        <v>165</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F87" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G86" t="s">
-        <v>4</v>
-      </c>
-      <c r="H86" t="s">
+      <c r="G87" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H87" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I86">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87">
+      <c r="I87" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="7">
         <v>100347</v>
       </c>
-      <c r="B87">
+      <c r="B88" s="2">
         <v>167</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C88" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D87">
+      <c r="D88" s="7">
         <v>167</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E88" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F88" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G88" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H87" t="s">
+      <c r="H88" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I87">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88">
+      <c r="I88" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="7">
         <v>153154</v>
       </c>
-      <c r="B88">
-        <v>165</v>
-      </c>
-      <c r="C88" s="1" t="s">
+      <c r="B89" s="2">
+        <v>165</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D88">
-        <v>165</v>
-      </c>
-      <c r="E88" t="s">
+      <c r="D89" s="7">
+        <v>165</v>
+      </c>
+      <c r="E89" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F89" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G88" t="s">
-        <v>4</v>
-      </c>
-      <c r="H88" t="s">
+      <c r="G89" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H89" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I88">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89">
+      <c r="I89" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="7">
         <v>152929</v>
       </c>
-      <c r="B89">
-        <v>165</v>
-      </c>
-      <c r="C89" s="1" t="s">
+      <c r="B90" s="2">
+        <v>165</v>
+      </c>
+      <c r="C90" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D89">
-        <v>165</v>
-      </c>
-      <c r="E89" t="s">
+      <c r="D90" s="7">
+        <v>165</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F89" t="s">
+      <c r="F90" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G89" t="s">
-        <v>4</v>
-      </c>
-      <c r="H89" t="s">
+      <c r="G90" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H90" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I89">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90">
+      <c r="I90" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="7">
         <v>151898</v>
       </c>
-      <c r="B90">
+      <c r="B91" s="2">
         <v>236</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C91" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D90">
+      <c r="D91" s="7">
         <v>236</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E91" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F91" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G91" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H90" t="s">
+      <c r="H91" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I90">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91">
+      <c r="I91" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="7">
         <v>120100</v>
       </c>
-      <c r="B91">
+      <c r="B92" s="2">
         <v>99</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C92" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D91">
+      <c r="D92" s="7">
         <v>99</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E92" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F91" t="s">
+      <c r="F92" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G92" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H91" t="s">
+      <c r="H92" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I91">
+      <c r="I92" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="7">
         <v>140105</v>
       </c>
-      <c r="B92">
+      <c r="B93" s="2">
         <v>167</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C93" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D92">
+      <c r="D93" s="7">
         <v>167</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E93" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F92" t="s">
+      <c r="F93" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G93" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H92" t="s">
+      <c r="H93" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I92">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93">
+      <c r="I93" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="7">
         <v>140440</v>
       </c>
-      <c r="B93">
+      <c r="B94" s="2">
         <v>207</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C94" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D93">
+      <c r="D94" s="7">
         <v>207</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E94" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F93" t="s">
+      <c r="F94" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G94" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H93" t="s">
+      <c r="H94" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I93">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94">
+      <c r="I94" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="7">
         <v>131712</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="B95" s="2"/>
+      <c r="C95" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D94" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95">
+      <c r="D95" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="2"/>
+      <c r="I95" s="16"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="7">
         <v>108058</v>
       </c>
-      <c r="B95">
+      <c r="B96" s="2">
         <v>99</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C96" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D95">
+      <c r="D96" s="7">
         <v>99</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E96" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F95" t="s">
+      <c r="F96" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G96" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H95" t="s">
+      <c r="H96" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I95">
+      <c r="I96" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="7">
         <v>128064</v>
       </c>
-      <c r="B96">
+      <c r="B97" s="2">
         <v>167</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C97" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D96">
+      <c r="D97" s="7">
         <v>167</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E97" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F96" t="s">
+      <c r="F97" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G96" t="s">
+      <c r="G97" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H96" t="s">
+      <c r="H97" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I96">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97">
+      <c r="I97" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="7">
         <v>103215</v>
       </c>
-      <c r="B97">
+      <c r="B98" s="2">
         <v>204</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C98" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D97">
+      <c r="D98" s="7">
         <v>204</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E98" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F97" t="s">
+      <c r="F98" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G97" t="s">
-        <v>4</v>
-      </c>
-      <c r="H97" t="s">
+      <c r="G98" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H98" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I97">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98">
+      <c r="I98" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="7">
         <v>124598</v>
       </c>
-      <c r="B98">
+      <c r="B99" s="2">
         <v>206</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C99" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D98">
+      <c r="D99" s="7">
         <v>206</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E99" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F98" t="s">
+      <c r="F99" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G99" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H98" t="s">
+      <c r="H99" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I98">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99">
+      <c r="I99" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="7">
         <v>51179</v>
       </c>
-      <c r="B99">
+      <c r="B100" s="2">
         <v>99</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C100" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D99">
+      <c r="D100" s="7">
         <v>99</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E100" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F99" t="s">
+      <c r="F100" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G100" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H99" t="s">
+      <c r="H100" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I99">
+      <c r="I100" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="7">
         <v>117514</v>
       </c>
-      <c r="B100">
+      <c r="B101" s="2">
         <v>167</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C101" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D100">
+      <c r="D101" s="7">
         <v>167</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E101" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F100" t="s">
+      <c r="F101" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G100" t="s">
+      <c r="G101" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H100" t="s">
+      <c r="H101" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I100">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101">
+      <c r="I101" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="8">
         <v>146577</v>
       </c>
-      <c r="B101">
+      <c r="B102" s="9">
         <v>182</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C102" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="D101">
+      <c r="D102" s="8">
         <v>182</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E102" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="F101" t="s">
+      <c r="F102" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="G101" t="s">
+      <c r="G102" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="H101" t="s">
+      <c r="H102" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="I101">
+      <c r="I102" s="17">
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:I1"/>
+  </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",D1)))</formula>

</xml_diff>